<commit_message>
update ets and bpaff to allow coal, nat gas to act as peakers
</commit_message>
<xml_diff>
--- a/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
+++ b/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
@@ -1,22 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipE\InputData\elec\BPaFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\South Korea\eps-southkorea\InputData\elec\BPaFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35822B4E-6402-4F94-BE56-6377A79E4D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="23955" windowHeight="10305"/>
+    <workbookView xWindow="1290" yWindow="1395" windowWidth="11700" windowHeight="12615" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BPaFF-BITPTaP" sheetId="2" r:id="rId2"/>
     <sheet name="BPaFF-BDTPTPF" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -152,7 +164,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -291,6 +303,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -326,6 +355,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -501,10 +547,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -647,7 +695,166 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <f>B2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <f>B6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <f>B11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16">
+        <f>B11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17">
+        <f>B9</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -801,161 +1008,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13">
-        <f>B2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14">
-        <f>B6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15">
-        <f>B11</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16">
-        <f>B11</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17">
-        <f>B9</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Draft elec sector edits
</commit_message>
<xml_diff>
--- a/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
+++ b/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
@@ -1,34 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\South Korea\eps-southkorea\InputData\elec\BPaFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipE\InputData\elec\BPaFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35822B4E-6402-4F94-BE56-6377A79E4D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="1395" windowWidth="11700" windowHeight="12615" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="23955" windowHeight="10305"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BPaFF-BITPTaP" sheetId="2" r:id="rId2"/>
     <sheet name="BPaFF-BDTPTPF" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -164,7 +152,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -303,23 +291,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -355,23 +326,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -547,12 +501,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -695,166 +647,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13">
-        <f>B2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14">
-        <f>B6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15">
-        <f>B11</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16">
-        <f>B11</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17">
-        <f>B9</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -1008,4 +801,161 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <f>B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <f>B6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <f>B11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16">
+        <f>B11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17">
+        <f>B9</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>